<commit_message>
fine tuned EE, ME, and added Transportation Engineering
</commit_message>
<xml_diff>
--- a/database/ComputerScience/CS_Course_database.xlsx
+++ b/database/ComputerScience/CS_Course_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B85856-1AA7-4CC0-A5AE-AF19577B991A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CAC879-6576-485E-B6D0-88B22C53DDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
     <sheet name="All_CS_Courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>離散數學</t>
   </si>
@@ -329,13 +329,313 @@
   </si>
   <si>
     <t>形式系統</t>
+  </si>
+  <si>
+    <t>所有科目_英語</t>
+  </si>
+  <si>
+    <t>Calculus (1)</t>
+  </si>
+  <si>
+    <t>Calculus (2)</t>
+  </si>
+  <si>
+    <t>Linear algebra</t>
+  </si>
+  <si>
+    <t>discrete mathematics</t>
+  </si>
+  <si>
+    <t>Computer organization</t>
+  </si>
+  <si>
+    <t>Software engineering</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Signal and system</t>
+  </si>
+  <si>
+    <t>Programming (1)</t>
+  </si>
+  <si>
+    <t>Programming (2)</t>
+  </si>
+  <si>
+    <t>Engineering Mathematics</t>
+  </si>
+  <si>
+    <t>Numerical Methods</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>Statistics (1)</t>
+  </si>
+  <si>
+    <t>Statistics (2)</t>
+  </si>
+  <si>
+    <t>Introduction to Computer (1)</t>
+  </si>
+  <si>
+    <t>Introduction to Computer (2)</t>
+  </si>
+  <si>
+    <t>General Physics (1)</t>
+  </si>
+  <si>
+    <t>General Physics (2)</t>
+  </si>
+  <si>
+    <t>Introduction to Neuroscience</t>
+  </si>
+  <si>
+    <t>Data science programming</t>
+  </si>
+  <si>
+    <t>Cross-platform application design</t>
+  </si>
+  <si>
+    <t>General Physics Experiment (1)</t>
+  </si>
+  <si>
+    <t>General Physics Experiment (2)</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Circuits</t>
+  </si>
+  <si>
+    <t>Introduction to Big Data</t>
+  </si>
+  <si>
+    <t>Digital circuit</t>
+  </si>
+  <si>
+    <t>Digital circuit experiment</t>
+  </si>
+  <si>
+    <t>System program</t>
+  </si>
+  <si>
+    <t>Web programming</t>
+  </si>
+  <si>
+    <t>Computer architecture</t>
+  </si>
+  <si>
+    <t>Unix programming</t>
+  </si>
+  <si>
+    <t>Data structure and algorithm (1)</t>
+  </si>
+  <si>
+    <t>Data structure and algorithm (2)</t>
+  </si>
+  <si>
+    <t>Computer Organization Experiment</t>
+  </si>
+  <si>
+    <t>working system</t>
+  </si>
+  <si>
+    <t>Operating system practice</t>
+  </si>
+  <si>
+    <t>Microcomputer experiment</t>
+  </si>
+  <si>
+    <t>Computer network</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (1)</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (2)</t>
+  </si>
+  <si>
+    <t>Object-oriented software design</t>
+  </si>
+  <si>
+    <t>Computer network experiment</t>
+  </si>
+  <si>
+    <t>Brain and behavior</t>
+  </si>
+  <si>
+    <t>Software and hardware topics (3)</t>
+  </si>
+  <si>
+    <t>Introduction to Multimedia Information</t>
+  </si>
+  <si>
+    <t>Network application software design</t>
+  </si>
+  <si>
+    <t>Introduction to Biomedical Information</t>
+  </si>
+  <si>
+    <t>Graph theory</t>
+  </si>
+  <si>
+    <t>Computability Theory</t>
+  </si>
+  <si>
+    <t>Formal system</t>
+  </si>
+  <si>
+    <t>Introduction to Formal Language</t>
+  </si>
+  <si>
+    <t>Basic graph theory</t>
+  </si>
+  <si>
+    <t>Random algorithm</t>
+  </si>
+  <si>
+    <t>Introduction to Machine Learning</t>
+  </si>
+  <si>
+    <t>Introduction to Compiler Design</t>
+  </si>
+  <si>
+    <t>Theoretical basis of machine learning algorithms</t>
+  </si>
+  <si>
+    <t>Introduction to Cryptography</t>
+  </si>
+  <si>
+    <t>Password engineering</t>
+  </si>
+  <si>
+    <t>Computer security</t>
+  </si>
+  <si>
+    <t>Communication principle</t>
+  </si>
+  <si>
+    <t>Wireless network</t>
+  </si>
+  <si>
+    <t>Total network system</t>
+  </si>
+  <si>
+    <t>Embedded Systems</t>
+  </si>
+  <si>
+    <t>Advanced Operating System</t>
+  </si>
+  <si>
+    <t>System effectiveness evaluation</t>
+  </si>
+  <si>
+    <t>Financial algorithm</t>
+  </si>
+  <si>
+    <t>Natural language processing</t>
+  </si>
+  <si>
+    <t>Software engineering design</t>
+  </si>
+  <si>
+    <t>Information Theory and Coding Skills</t>
+  </si>
+  <si>
+    <t>Higher Computer Network</t>
+  </si>
+  <si>
+    <t>Higher computer architecture</t>
+  </si>
+  <si>
+    <t>Parallel programming</t>
+  </si>
+  <si>
+    <t>Multimedia Information System</t>
+  </si>
+  <si>
+    <t>Digital image processing</t>
+  </si>
+  <si>
+    <t>Artificial intelligence</t>
+  </si>
+  <si>
+    <t>Graphics Algorithm Features</t>
+  </si>
+  <si>
+    <t>Medical Information System</t>
+  </si>
+  <si>
+    <t>Cryptography and Information Security</t>
+  </si>
+  <si>
+    <t>Digital visual effects</t>
+  </si>
+  <si>
+    <t>Game theory</t>
+  </si>
+  <si>
+    <t>Internet Information Retrieval and Exploration</t>
+  </si>
+  <si>
+    <t>Advanced human-computer interaction interface</t>
+  </si>
+  <si>
+    <t>Advanced Computer Vision</t>
+  </si>
+  <si>
+    <t>Massive data system</t>
+  </si>
+  <si>
+    <t>Virtual machine</t>
+  </si>
+  <si>
+    <t>Smart networking topics</t>
+  </si>
+  <si>
+    <t>Introduction to Mathematical Logic</t>
+  </si>
+  <si>
+    <t>Human Machine Interface and Design</t>
+  </si>
+  <si>
+    <t>Application of deep learning</t>
+  </si>
+  <si>
+    <t>Introduction to Communication Complexity</t>
+  </si>
+  <si>
+    <t>Introduction to Blockchain</t>
+  </si>
+  <si>
+    <t>High-performance artificial intelligence system</t>
+  </si>
+  <si>
+    <t>Predict, learn, and match</t>
+  </si>
+  <si>
+    <t>Advanced Interactive Technology</t>
+  </si>
+  <si>
+    <t>Introduction to Safety Program Development</t>
+  </si>
+  <si>
+    <t>System and network security experiment</t>
+  </si>
+  <si>
+    <t>Functional programming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,8 +686,25 @@
       <family val="4"/>
       <charset val="136"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Linux Libertine G"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Linux Libertine G"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,8 +717,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -424,6 +747,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -433,7 +771,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -472,6 +810,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -790,21 +1143,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
   <dimension ref="A1:W425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21.09765625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.796875" style="1"/>
+    <col min="2" max="2" width="22.8984375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:23" ht="16.2" thickBot="1">
+      <c r="A1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -825,12 +1181,14 @@
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="16.2" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="14"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="H2" s="6"/>
@@ -850,12 +1208,14 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" ht="16.2" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="H3" s="6"/>
@@ -875,12 +1235,14 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" ht="16.2" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="14"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="H4" s="6"/>
@@ -900,12 +1262,14 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" ht="16.2">
+    <row r="5" spans="1:23" ht="16.8" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="14"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="H5" s="6"/>
@@ -925,12 +1289,14 @@
       <c r="V5" s="6"/>
       <c r="W5" s="8"/>
     </row>
-    <row r="6" spans="1:23" ht="16.2">
+    <row r="6" spans="1:23" ht="16.8" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="14"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="H6" s="6"/>
@@ -950,12 +1316,14 @@
       <c r="V6" s="6"/>
       <c r="W6" s="8"/>
     </row>
-    <row r="7" spans="1:23" ht="16.2">
+    <row r="7" spans="1:23" ht="30.6" thickBot="1">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="H7" s="6"/>
@@ -975,11 +1343,14 @@
       <c r="V7" s="6"/>
       <c r="W7" s="8"/>
     </row>
-    <row r="8" spans="1:23" ht="16.2">
+    <row r="8" spans="1:23" ht="16.8" thickBot="1">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="H8" s="6"/>
@@ -1003,7 +1374,10 @@
       <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="H9" s="6"/>
@@ -1023,11 +1397,14 @@
       <c r="V9" s="2"/>
       <c r="W9" s="8"/>
     </row>
-    <row r="10" spans="1:23" ht="16.2">
+    <row r="10" spans="1:23" ht="16.8" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="H10" s="6"/>
@@ -1047,11 +1424,14 @@
       <c r="V10" s="2"/>
       <c r="W10" s="8"/>
     </row>
-    <row r="11" spans="1:23" ht="16.2">
+    <row r="11" spans="1:23" ht="16.8" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="H11" s="6"/>
@@ -1071,11 +1451,14 @@
       <c r="V11" s="2"/>
       <c r="W11" s="8"/>
     </row>
-    <row r="12" spans="1:23" ht="16.2">
+    <row r="12" spans="1:23" ht="16.8" thickBot="1">
       <c r="A12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="H12" s="6"/>
@@ -1095,11 +1478,14 @@
       <c r="V12" s="2"/>
       <c r="W12" s="8"/>
     </row>
-    <row r="13" spans="1:23" ht="16.2">
+    <row r="13" spans="1:23" ht="30.6" thickBot="1">
       <c r="A13" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="H13" s="6"/>
@@ -1119,11 +1505,14 @@
       <c r="V13" s="2"/>
       <c r="W13" s="8"/>
     </row>
-    <row r="14" spans="1:23" ht="16.2">
+    <row r="14" spans="1:23" ht="30.6" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="14"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="H14" s="6"/>
@@ -1143,11 +1532,14 @@
       <c r="V14" s="2"/>
       <c r="W14" s="8"/>
     </row>
-    <row r="15" spans="1:23" ht="16.2">
+    <row r="15" spans="1:23" ht="16.8" thickBot="1">
       <c r="A15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="H15" s="6"/>
@@ -1167,11 +1559,14 @@
       <c r="V15" s="2"/>
       <c r="W15" s="8"/>
     </row>
-    <row r="16" spans="1:23" ht="16.2">
+    <row r="16" spans="1:23" ht="16.8" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="H16" s="6"/>
@@ -1191,11 +1586,14 @@
       <c r="V16" s="2"/>
       <c r="W16" s="8"/>
     </row>
-    <row r="17" spans="1:23" ht="16.2">
+    <row r="17" spans="1:23" ht="30.6" thickBot="1">
       <c r="A17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="H17" s="6"/>
@@ -1215,11 +1613,14 @@
       <c r="V17" s="2"/>
       <c r="W17" s="8"/>
     </row>
-    <row r="18" spans="1:23" ht="16.2">
+    <row r="18" spans="1:23" ht="30.6" thickBot="1">
       <c r="A18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="14"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="H18" s="6"/>
@@ -1239,11 +1640,14 @@
       <c r="V18" s="2"/>
       <c r="W18" s="8"/>
     </row>
-    <row r="19" spans="1:23" ht="16.2">
+    <row r="19" spans="1:23" ht="30.6" thickBot="1">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="14"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="H19" s="6"/>
@@ -1263,11 +1667,14 @@
       <c r="V19" s="2"/>
       <c r="W19" s="8"/>
     </row>
-    <row r="20" spans="1:23" ht="16.2">
+    <row r="20" spans="1:23" ht="30.6" thickBot="1">
       <c r="A20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="14"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="H20" s="6"/>
@@ -1287,11 +1694,14 @@
       <c r="V20" s="2"/>
       <c r="W20" s="8"/>
     </row>
-    <row r="21" spans="1:23" ht="16.2">
+    <row r="21" spans="1:23" ht="30.6" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="14"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="H21" s="6"/>
@@ -1311,11 +1721,14 @@
       <c r="V21" s="2"/>
       <c r="W21" s="8"/>
     </row>
-    <row r="22" spans="1:23" ht="16.2">
+    <row r="22" spans="1:23" ht="16.8" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="14"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="H22" s="6"/>
@@ -1335,11 +1748,14 @@
       <c r="V22" s="2"/>
       <c r="W22" s="8"/>
     </row>
-    <row r="23" spans="1:23" ht="16.2">
+    <row r="23" spans="1:23" ht="16.8" thickBot="1">
       <c r="A23" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="14"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="H23" s="6"/>
@@ -1359,11 +1775,14 @@
       <c r="V23" s="2"/>
       <c r="W23" s="8"/>
     </row>
-    <row r="24" spans="1:23" ht="16.2">
+    <row r="24" spans="1:23" ht="16.8" thickBot="1">
       <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="14"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="H24" s="6"/>
@@ -1383,11 +1802,14 @@
       <c r="V24" s="2"/>
       <c r="W24" s="8"/>
     </row>
-    <row r="25" spans="1:23" ht="16.2">
+    <row r="25" spans="1:23" ht="16.8" thickBot="1">
       <c r="A25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="14"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="H25" s="6"/>
@@ -1407,11 +1829,14 @@
       <c r="V25" s="2"/>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="1:23" ht="16.2">
+    <row r="26" spans="1:23" ht="16.8" thickBot="1">
       <c r="A26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="14"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="H26" s="6"/>
@@ -1431,11 +1856,14 @@
       <c r="V26" s="2"/>
       <c r="W26" s="8"/>
     </row>
-    <row r="27" spans="1:23" ht="16.2">
+    <row r="27" spans="1:23" ht="16.8" thickBot="1">
       <c r="A27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="14"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="H27" s="6"/>
@@ -1455,11 +1883,14 @@
       <c r="V27" s="2"/>
       <c r="W27" s="8"/>
     </row>
-    <row r="28" spans="1:23" ht="16.2">
+    <row r="28" spans="1:23" ht="16.8" thickBot="1">
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="14"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="H28" s="6"/>
@@ -1479,11 +1910,14 @@
       <c r="V28" s="6"/>
       <c r="W28" s="8"/>
     </row>
-    <row r="29" spans="1:23" ht="16.2">
+    <row r="29" spans="1:23" ht="16.8" thickBot="1">
       <c r="A29" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="14"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="H29" s="6"/>
@@ -1503,11 +1937,14 @@
       <c r="V29" s="6"/>
       <c r="W29" s="8"/>
     </row>
-    <row r="30" spans="1:23" ht="16.2">
+    <row r="30" spans="1:23" ht="16.8" thickBot="1">
       <c r="A30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="14"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="H30" s="6"/>
@@ -1527,11 +1964,14 @@
       <c r="V30" s="2"/>
       <c r="W30" s="8"/>
     </row>
-    <row r="31" spans="1:23" ht="16.2">
+    <row r="31" spans="1:23" ht="16.8" thickBot="1">
       <c r="A31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="14"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="H31" s="6"/>
@@ -1551,11 +1991,14 @@
       <c r="V31" s="2"/>
       <c r="W31" s="8"/>
     </row>
-    <row r="32" spans="1:23" ht="16.2">
+    <row r="32" spans="1:23" ht="16.8" thickBot="1">
       <c r="A32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="14"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="H32" s="6"/>
@@ -1575,11 +2018,14 @@
       <c r="V32" s="2"/>
       <c r="W32" s="8"/>
     </row>
-    <row r="33" spans="1:23" ht="16.2">
+    <row r="33" spans="1:23" ht="30.6" thickBot="1">
       <c r="A33" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="14"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="H33" s="6"/>
@@ -1599,11 +2045,14 @@
       <c r="V33" s="2"/>
       <c r="W33" s="8"/>
     </row>
-    <row r="34" spans="1:23" ht="16.2">
+    <row r="34" spans="1:23" ht="30.6" thickBot="1">
       <c r="A34" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="14"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="H34" s="6"/>
@@ -1623,11 +2072,14 @@
       <c r="V34" s="2"/>
       <c r="W34" s="8"/>
     </row>
-    <row r="35" spans="1:23" ht="16.2">
+    <row r="35" spans="1:23" ht="30.6" thickBot="1">
       <c r="A35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="14"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="H35" s="6"/>
@@ -1647,11 +2099,14 @@
       <c r="V35" s="2"/>
       <c r="W35" s="8"/>
     </row>
-    <row r="36" spans="1:23" ht="16.2">
+    <row r="36" spans="1:23" ht="16.8" thickBot="1">
       <c r="A36" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="14"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="H36" s="6"/>
@@ -1671,11 +2126,14 @@
       <c r="V36" s="2"/>
       <c r="W36" s="8"/>
     </row>
-    <row r="37" spans="1:23" ht="16.2">
+    <row r="37" spans="1:23" ht="30.6" thickBot="1">
       <c r="A37" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="6"/>
+      <c r="B37" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="14"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="H37" s="6"/>
@@ -1695,11 +2153,14 @@
       <c r="V37" s="2"/>
       <c r="W37" s="8"/>
     </row>
-    <row r="38" spans="1:23" ht="16.2">
+    <row r="38" spans="1:23" ht="30.6" thickBot="1">
       <c r="A38" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="14"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="H38" s="6"/>
@@ -1719,11 +2180,14 @@
       <c r="V38" s="2"/>
       <c r="W38" s="8"/>
     </row>
-    <row r="39" spans="1:23" ht="16.2">
+    <row r="39" spans="1:23" ht="16.8" thickBot="1">
       <c r="A39" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="14"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="H39" s="6"/>
@@ -1743,11 +2207,14 @@
       <c r="V39" s="2"/>
       <c r="W39" s="8"/>
     </row>
-    <row r="40" spans="1:23" ht="16.2">
+    <row r="40" spans="1:23" ht="16.8" thickBot="1">
       <c r="A40" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="6"/>
+      <c r="B40" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="14"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="H40" s="6"/>
@@ -1767,11 +2234,14 @@
       <c r="V40" s="2"/>
       <c r="W40" s="8"/>
     </row>
-    <row r="41" spans="1:23" ht="16.2">
+    <row r="41" spans="1:23" ht="30.6" thickBot="1">
       <c r="A41" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="6"/>
+      <c r="B41" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="14"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="H41" s="6"/>
@@ -1791,11 +2261,14 @@
       <c r="V41" s="2"/>
       <c r="W41" s="8"/>
     </row>
-    <row r="42" spans="1:23" ht="16.2">
+    <row r="42" spans="1:23" ht="30.6" thickBot="1">
       <c r="A42" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="6"/>
+      <c r="B42" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="14"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="H42" s="6"/>
@@ -1815,11 +2288,14 @@
       <c r="V42" s="6"/>
       <c r="W42" s="8"/>
     </row>
-    <row r="43" spans="1:23" ht="16.2">
+    <row r="43" spans="1:23" ht="30.6" thickBot="1">
       <c r="A43" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="6"/>
+      <c r="B43" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="14"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="H43" s="6"/>
@@ -1839,11 +2315,14 @@
       <c r="V43" s="6"/>
       <c r="W43" s="8"/>
     </row>
-    <row r="44" spans="1:23" ht="16.2">
+    <row r="44" spans="1:23" ht="30.6" thickBot="1">
       <c r="A44" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="14"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="H44" s="6"/>
@@ -1863,11 +2342,14 @@
       <c r="V44" s="2"/>
       <c r="W44" s="8"/>
     </row>
-    <row r="45" spans="1:23" ht="16.2">
+    <row r="45" spans="1:23" ht="16.8" thickBot="1">
       <c r="A45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="14"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="H45" s="6"/>
@@ -1887,11 +2369,14 @@
       <c r="V45" s="6"/>
       <c r="W45" s="8"/>
     </row>
-    <row r="46" spans="1:23" ht="16.2">
+    <row r="46" spans="1:23" ht="30.6" thickBot="1">
       <c r="A46" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="14"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="H46" s="6"/>
@@ -1911,11 +2396,14 @@
       <c r="V46" s="6"/>
       <c r="W46" s="8"/>
     </row>
-    <row r="47" spans="1:23" ht="16.2">
+    <row r="47" spans="1:23" ht="30.6" thickBot="1">
       <c r="A47" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="H47" s="6"/>
@@ -1935,11 +2423,14 @@
       <c r="V47" s="6"/>
       <c r="W47" s="8"/>
     </row>
-    <row r="48" spans="1:23" ht="16.2">
+    <row r="48" spans="1:23" ht="30.6" thickBot="1">
       <c r="A48" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="14"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="H48" s="6"/>
@@ -1959,11 +2450,14 @@
       <c r="V48" s="6"/>
       <c r="W48" s="8"/>
     </row>
-    <row r="49" spans="1:23" ht="16.2">
+    <row r="49" spans="1:23" ht="30.6" thickBot="1">
       <c r="A49" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="14"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="H49" s="6"/>
@@ -1987,7 +2481,10 @@
       <c r="A50" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="14"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="H50" s="6"/>
@@ -2011,7 +2508,10 @@
       <c r="A51" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="14"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="H51" s="6"/>
@@ -2035,7 +2535,10 @@
       <c r="A52" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="14"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="H52" s="6"/>
@@ -2055,11 +2558,14 @@
       <c r="V52" s="2"/>
       <c r="W52" s="8"/>
     </row>
-    <row r="53" spans="1:23" ht="16.2">
+    <row r="53" spans="1:23" ht="30">
       <c r="A53" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="6"/>
+      <c r="B53" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="14"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="H53" s="6"/>
@@ -2083,7 +2589,10 @@
       <c r="A54" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="6"/>
+      <c r="B54" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="14"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="H54" s="6"/>
@@ -2107,7 +2616,10 @@
       <c r="A55" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="6"/>
+      <c r="B55" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="H55" s="6"/>
@@ -2127,11 +2639,14 @@
       <c r="V55" s="2"/>
       <c r="W55" s="8"/>
     </row>
-    <row r="56" spans="1:23" ht="16.2">
+    <row r="56" spans="1:23" ht="30">
       <c r="A56" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B56" s="6"/>
+      <c r="B56" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="H56" s="6"/>
@@ -2151,11 +2666,14 @@
       <c r="V56" s="2"/>
       <c r="W56" s="8"/>
     </row>
-    <row r="57" spans="1:23" ht="16.2">
+    <row r="57" spans="1:23" ht="30">
       <c r="A57" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="6"/>
+      <c r="B57" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="14"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="H57" s="6"/>
@@ -2175,11 +2693,14 @@
       <c r="V57" s="2"/>
       <c r="W57" s="8"/>
     </row>
-    <row r="58" spans="1:23" ht="16.2">
+    <row r="58" spans="1:23" ht="45">
       <c r="A58" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="14"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="H58" s="6"/>
@@ -2199,11 +2720,14 @@
       <c r="V58" s="2"/>
       <c r="W58" s="8"/>
     </row>
-    <row r="59" spans="1:23" ht="16.2">
+    <row r="59" spans="1:23" ht="30">
       <c r="A59" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B59" s="6"/>
+      <c r="B59" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="14"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="H59" s="6"/>
@@ -2227,7 +2751,10 @@
       <c r="A60" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="14"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="H60" s="6"/>
@@ -2251,7 +2778,10 @@
       <c r="A61" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="6"/>
+      <c r="B61" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="14"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="H61" s="6"/>
@@ -2275,7 +2805,10 @@
       <c r="A62" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="14"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="H62" s="6"/>
@@ -2299,7 +2832,10 @@
       <c r="A63" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="6"/>
+      <c r="B63" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="14"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="H63" s="6"/>
@@ -2323,7 +2859,10 @@
       <c r="A64" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="6"/>
+      <c r="B64" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="14"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="H64" s="6"/>
@@ -2347,7 +2886,10 @@
       <c r="A65" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="6"/>
+      <c r="B65" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="14"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="H65" s="6"/>
@@ -2367,11 +2909,14 @@
       <c r="V65" s="6"/>
       <c r="W65" s="8"/>
     </row>
-    <row r="66" spans="1:23" ht="16.2">
+    <row r="66" spans="1:23" ht="30">
       <c r="A66" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B66" s="6"/>
+      <c r="B66" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="14"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="H66" s="6"/>
@@ -2391,11 +2936,14 @@
       <c r="V66" s="6"/>
       <c r="W66" s="8"/>
     </row>
-    <row r="67" spans="1:23" ht="16.2">
+    <row r="67" spans="1:23" ht="30">
       <c r="A67" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B67" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="14"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="H67" s="6"/>
@@ -2419,7 +2967,10 @@
       <c r="A68" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="6"/>
+      <c r="B68" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="14"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="H68" s="6"/>
@@ -2439,11 +2990,14 @@
       <c r="V68" s="6"/>
       <c r="W68" s="8"/>
     </row>
-    <row r="69" spans="1:23" ht="16.2">
+    <row r="69" spans="1:23" ht="30">
       <c r="A69" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B69" s="6"/>
+      <c r="B69" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C69" s="14"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="H69" s="6"/>
@@ -2463,11 +3017,14 @@
       <c r="V69" s="6"/>
       <c r="W69" s="8"/>
     </row>
-    <row r="70" spans="1:23" ht="16.2">
+    <row r="70" spans="1:23" ht="30">
       <c r="A70" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B70" s="6"/>
+      <c r="B70" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" s="14"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="H70" s="6"/>
@@ -2487,11 +3044,14 @@
       <c r="V70" s="6"/>
       <c r="W70" s="8"/>
     </row>
-    <row r="71" spans="1:23" ht="16.2">
+    <row r="71" spans="1:23" ht="30">
       <c r="A71" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B71" s="6"/>
+      <c r="B71" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" s="14"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="H71" s="6"/>
@@ -2511,11 +3071,14 @@
       <c r="V71" s="6"/>
       <c r="W71" s="8"/>
     </row>
-    <row r="72" spans="1:23" ht="16.2">
+    <row r="72" spans="1:23" ht="30">
       <c r="A72" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B72" s="6"/>
+      <c r="B72" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C72" s="14"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="H72" s="6"/>
@@ -2535,11 +3098,14 @@
       <c r="V72" s="6"/>
       <c r="W72" s="8"/>
     </row>
-    <row r="73" spans="1:23" ht="16.2">
+    <row r="73" spans="1:23" ht="30">
       <c r="A73" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="6"/>
+      <c r="B73" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C73" s="14"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="H73" s="6"/>
@@ -2563,7 +3129,10 @@
       <c r="A74" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B74" s="6"/>
+      <c r="B74" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C74" s="14"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="H74" s="6"/>
@@ -2583,11 +3152,14 @@
       <c r="V74" s="6"/>
       <c r="W74" s="8"/>
     </row>
-    <row r="75" spans="1:23" ht="16.2">
+    <row r="75" spans="1:23" ht="30">
       <c r="A75" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="14"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="H75" s="6"/>
@@ -2611,7 +3183,10 @@
       <c r="A76" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="14"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="H76" s="6"/>
@@ -2635,7 +3210,10 @@
       <c r="A77" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B77" s="6"/>
+      <c r="B77" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="14"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="H77" s="6"/>
@@ -2655,11 +3233,14 @@
       <c r="V77" s="6"/>
       <c r="W77" s="8"/>
     </row>
-    <row r="78" spans="1:23" ht="16.2">
+    <row r="78" spans="1:23" ht="30">
       <c r="A78" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B78" s="6"/>
+      <c r="B78" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="14"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="H78" s="6"/>
@@ -2679,11 +3260,14 @@
       <c r="V78" s="2"/>
       <c r="W78" s="8"/>
     </row>
-    <row r="79" spans="1:23" ht="16.2">
+    <row r="79" spans="1:23" ht="30">
       <c r="A79" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C79" s="14"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="H79" s="6"/>
@@ -2703,11 +3287,14 @@
       <c r="V79" s="2"/>
       <c r="W79" s="8"/>
     </row>
-    <row r="80" spans="1:23" ht="16.2">
+    <row r="80" spans="1:23" ht="30">
       <c r="A80" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B80" s="6"/>
+      <c r="B80" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="14"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="H80" s="6"/>
@@ -2731,7 +3318,10 @@
       <c r="A81" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B81" s="6"/>
+      <c r="B81" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C81" s="14"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="H81" s="6"/>
@@ -2755,7 +3345,10 @@
       <c r="A82" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B82" s="6"/>
+      <c r="B82" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="14"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="H82" s="6"/>
@@ -2775,11 +3368,14 @@
       <c r="V82" s="6"/>
       <c r="W82" s="8"/>
     </row>
-    <row r="83" spans="1:23" ht="16.2">
+    <row r="83" spans="1:23" ht="45">
       <c r="A83" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B83" s="6"/>
+      <c r="B83" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" s="14"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="H83" s="6"/>
@@ -2799,11 +3395,14 @@
       <c r="V83" s="6"/>
       <c r="W83" s="8"/>
     </row>
-    <row r="84" spans="1:23" ht="16.2">
+    <row r="84" spans="1:23" ht="45">
       <c r="A84" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B84" s="6"/>
+      <c r="B84" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="14"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="H84" s="6"/>
@@ -2823,11 +3422,14 @@
       <c r="V84" s="2"/>
       <c r="W84" s="8"/>
     </row>
-    <row r="85" spans="1:23" ht="16.2">
+    <row r="85" spans="1:23" ht="30">
       <c r="A85" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B85" s="6"/>
+      <c r="B85" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="14"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="H85" s="6"/>
@@ -2851,7 +3453,10 @@
       <c r="A86" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="B86" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="C86" s="14"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="H86" s="6"/>
@@ -2875,7 +3480,10 @@
       <c r="A87" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B87" s="6"/>
+      <c r="B87" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" s="14"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
       <c r="H87" s="6"/>
@@ -2899,7 +3507,10 @@
       <c r="A88" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B88" s="6"/>
+      <c r="B88" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="14"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="H88" s="6"/>
@@ -2919,11 +3530,14 @@
       <c r="V88" s="6"/>
       <c r="W88" s="8"/>
     </row>
-    <row r="89" spans="1:23" ht="16.2">
+    <row r="89" spans="1:23" ht="30">
       <c r="A89" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B89" s="6"/>
+      <c r="B89" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" s="14"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
       <c r="H89" s="6"/>
@@ -2943,11 +3557,14 @@
       <c r="V89" s="6"/>
       <c r="W89" s="8"/>
     </row>
-    <row r="90" spans="1:23" ht="16.2">
+    <row r="90" spans="1:23" ht="30">
       <c r="A90" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B90" s="6"/>
+      <c r="B90" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="14"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
       <c r="H90" s="6"/>
@@ -2967,11 +3584,14 @@
       <c r="V90" s="6"/>
       <c r="W90" s="8"/>
     </row>
-    <row r="91" spans="1:23" ht="16.2">
+    <row r="91" spans="1:23" ht="30">
       <c r="A91" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B91" s="6"/>
+      <c r="B91" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C91" s="14"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="H91" s="6"/>
@@ -2991,11 +3611,14 @@
       <c r="V91" s="6"/>
       <c r="W91" s="8"/>
     </row>
-    <row r="92" spans="1:23" ht="16.2">
+    <row r="92" spans="1:23" ht="45">
       <c r="A92" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B92" s="6"/>
+      <c r="B92" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" s="14"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
       <c r="H92" s="6"/>
@@ -3015,11 +3638,14 @@
       <c r="V92" s="6"/>
       <c r="W92" s="8"/>
     </row>
-    <row r="93" spans="1:23" ht="16.2">
+    <row r="93" spans="1:23" ht="30">
       <c r="A93" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B93" s="6"/>
+      <c r="B93" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C93" s="14"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
       <c r="H93" s="6"/>
@@ -3039,11 +3665,14 @@
       <c r="V93" s="6"/>
       <c r="W93" s="8"/>
     </row>
-    <row r="94" spans="1:23" ht="16.2">
+    <row r="94" spans="1:23" ht="45">
       <c r="A94" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B94" s="6"/>
+      <c r="B94" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" s="14"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
       <c r="H94" s="6"/>
@@ -3063,11 +3692,14 @@
       <c r="V94" s="6"/>
       <c r="W94" s="8"/>
     </row>
-    <row r="95" spans="1:23" ht="16.2">
+    <row r="95" spans="1:23" ht="30">
       <c r="A95" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B95" s="6"/>
+      <c r="B95" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C95" s="14"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
       <c r="H95" s="6"/>
@@ -3087,11 +3719,14 @@
       <c r="V95" s="6"/>
       <c r="W95" s="8"/>
     </row>
-    <row r="96" spans="1:23" ht="16.2">
+    <row r="96" spans="1:23" ht="30">
       <c r="A96" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="6"/>
+      <c r="B96" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C96" s="14"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="H96" s="6"/>
@@ -3111,12 +3746,14 @@
       <c r="V96" s="6"/>
       <c r="W96" s="8"/>
     </row>
-    <row r="97" spans="1:23" ht="16.2">
+    <row r="97" spans="1:23" ht="30">
       <c r="A97" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
+      <c r="B97" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="14"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="H97" s="6"/>
@@ -3136,12 +3773,14 @@
       <c r="V97" s="6"/>
       <c r="W97" s="8"/>
     </row>
-    <row r="98" spans="1:23" ht="16.2">
+    <row r="98" spans="1:23" ht="30">
       <c r="A98" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
+      <c r="B98" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C98" s="14"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="H98" s="6"/>
@@ -3165,8 +3804,10 @@
       <c r="A99" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B99" s="6"/>
-      <c r="C99" s="6"/>
+      <c r="B99" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="14"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
       <c r="H99" s="6"/>
@@ -3190,8 +3831,10 @@
       <c r="A100" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
+      <c r="B100" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100"/>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
       <c r="H100" s="6"/>

</xml_diff>